<commit_message>
more figure updates and correct raster fig dims
</commit_message>
<xml_diff>
--- a/tort_report_figures/all_rasters_table.xlsx
+++ b/tort_report_figures/all_rasters_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="0" windowWidth="17960" windowHeight="15220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6640" yWindow="0" windowWidth="24960" windowHeight="16320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_raster_info" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="566">
   <si>
     <t>layer name</t>
   </si>
@@ -1725,7 +1725,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1759,6 +1759,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1780,7 +1786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1853,12 +1859,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1897,14 +1932,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1928,8 +1957,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2263,11 +2303,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2277,13 +2317,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="17" customFormat="1" ht="37" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="33" t="s">
         <v>531</v>
       </c>
     </row>
@@ -2291,10 +2331,10 @@
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>537</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="35" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2305,7 +2345,7 @@
       <c r="B3" s="15" t="s">
         <v>534</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2334,7 +2374,7 @@
       <c r="B6" s="15" t="s">
         <v>538</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2354,7 +2394,7 @@
       <c r="B8" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2365,7 +2405,7 @@
       <c r="B9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2385,7 +2425,7 @@
       <c r="B11" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2396,7 +2436,7 @@
       <c r="B12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2659,7 +2699,7 @@
       <c r="B41" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="26"/>
+      <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
       <c r="A42" s="19" t="s">
@@ -2668,7 +2708,7 @@
       <c r="B42" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="26"/>
+      <c r="C42" s="24"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
@@ -2677,7 +2717,7 @@
       <c r="B43" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="24"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="A44" s="19" t="s">
@@ -2686,7 +2726,7 @@
       <c r="B44" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="26"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
@@ -2695,7 +2735,7 @@
       <c r="B45" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="24"/>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
@@ -2704,7 +2744,7 @@
       <c r="B46" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="A47" s="19" t="s">
@@ -2713,7 +2753,7 @@
       <c r="B47" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="26"/>
+      <c r="C47" s="24"/>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
@@ -2722,7 +2762,7 @@
       <c r="B48" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="24"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
@@ -2731,7 +2771,7 @@
       <c r="B49" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="26"/>
+      <c r="C49" s="24"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
@@ -2740,7 +2780,7 @@
       <c r="B50" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="26"/>
+      <c r="C50" s="24"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
@@ -2749,7 +2789,7 @@
       <c r="B51" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="24"/>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1">
       <c r="A52" s="19" t="s">
@@ -2758,7 +2798,7 @@
       <c r="B52" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="26"/>
+      <c r="C52" s="24"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1">
       <c r="A53" s="19" t="s">
@@ -2767,7 +2807,7 @@
       <c r="B53" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="26"/>
+      <c r="C53" s="24"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" customHeight="1">
       <c r="A54" s="19" t="s">
@@ -2776,7 +2816,7 @@
       <c r="B54" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="26"/>
+      <c r="C54" s="24"/>
     </row>
     <row r="55" spans="1:3" ht="15.75" customHeight="1">
       <c r="A55" s="19" t="s">
@@ -2785,7 +2825,7 @@
       <c r="B55" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="26"/>
+      <c r="C55" s="24"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
@@ -2794,7 +2834,7 @@
       <c r="B56" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="26"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
@@ -2803,7 +2843,7 @@
       <c r="B57" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="26"/>
+      <c r="C57" s="24"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
       <c r="A58" s="19" t="s">
@@ -2812,7 +2852,7 @@
       <c r="B58" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="26"/>
+      <c r="C58" s="24"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
@@ -2821,7 +2861,7 @@
       <c r="B59" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="26"/>
+      <c r="C59" s="24"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
@@ -2830,7 +2870,7 @@
       <c r="B60" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="26"/>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
@@ -2839,7 +2879,7 @@
       <c r="B61" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="26"/>
+      <c r="C61" s="24"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
@@ -2848,7 +2888,7 @@
       <c r="B62" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="26"/>
+      <c r="C62" s="24"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
@@ -2857,7 +2897,7 @@
       <c r="B63" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="26"/>
+      <c r="C63" s="24"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
@@ -2866,7 +2906,7 @@
       <c r="B64" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="25" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2877,7 +2917,7 @@
       <c r="B65" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="26"/>
+      <c r="C65" s="24"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
@@ -2886,7 +2926,7 @@
       <c r="B66" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="26"/>
+      <c r="C66" s="24"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" customHeight="1">
       <c r="A67" s="19" t="s">
@@ -2895,7 +2935,7 @@
       <c r="B67" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="26"/>
+      <c r="C67" s="24"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" customHeight="1">
       <c r="A68" s="19" t="s">
@@ -2913,7 +2953,7 @@
       <c r="B69" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -2942,7 +2982,7 @@
       <c r="B72" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C72" s="25" t="s">
+      <c r="C72" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -3016,7 +3056,7 @@
       <c r="B80" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="23" t="s">
         <v>558</v>
       </c>
     </row>
@@ -3038,24 +3078,35 @@
       </c>
       <c r="C82" s="21"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A83" s="20" t="s">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A83" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>548</v>
       </c>
-      <c r="C83" s="22"/>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A84" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" s="34" t="s">
+        <v>555</v>
+      </c>
+      <c r="C84" s="36" t="s">
+        <v>558</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="49" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="48" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="26" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="7" max="1048575" man="1"/>
+    <brk id="6" max="1048575" man="1"/>
   </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3070,7 +3121,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3082,25 +3133,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="31" t="s">
         <v>560</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="31" t="s">
         <v>565</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="31" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3111,17 +3162,17 @@
       <c r="B2" s="15" t="s">
         <v>561</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3135,12 +3186,12 @@
       <c r="C3" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3154,16 +3205,16 @@
       <c r="C4" s="15" t="s">
         <v>534</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3177,10 +3228,10 @@
       <c r="C5" s="15" t="s">
         <v>535</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3194,12 +3245,12 @@
       <c r="C6" s="15" t="s">
         <v>536</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3213,12 +3264,12 @@
       <c r="C7" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3232,16 +3283,16 @@
       <c r="C8" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3255,10 +3306,10 @@
       <c r="C9" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3272,12 +3323,12 @@
       <c r="C10" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3291,10 +3342,10 @@
       <c r="C11" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3308,10 +3359,12 @@
       <c r="C12" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25" t="s">
+      <c r="D12" s="23" t="s">
+        <v>558</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3325,16 +3378,16 @@
       <c r="C13" s="15" t="s">
         <v>537</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3348,12 +3401,12 @@
       <c r="C14" s="15" t="s">
         <v>538</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3367,10 +3420,10 @@
       <c r="C15" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3384,16 +3437,16 @@
       <c r="C16" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3407,12 +3460,12 @@
       <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25" t="s">
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3426,10 +3479,10 @@
       <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25" t="s">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3443,10 +3496,10 @@
       <c r="C19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25" t="s">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3460,10 +3513,10 @@
       <c r="C20" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25" t="s">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3477,12 +3530,12 @@
       <c r="C21" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25" t="s">
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3496,10 +3549,10 @@
       <c r="C22" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25" t="s">
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3513,14 +3566,14 @@
       <c r="C23" s="15" t="s">
         <v>563</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3534,16 +3587,16 @@
       <c r="C24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3557,33 +3610,33 @@
       <c r="C25" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="23" t="s">
         <v>558</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25" t="s">
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="23" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13" thickBot="1">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29" t="s">
         <v>564</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32">
+      <c r="D26" s="30"/>
+      <c r="E26" s="30">
         <f>COUNTIF(E2:E25,"x")</f>
         <v>6</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="30">
         <f>COUNTIF(F2:F25,"x")</f>
         <v>12</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="30">
         <f>COUNTIF(G2:G25,"x")</f>
         <v>24</v>
       </c>
@@ -3605,7 +3658,7 @@
   <dimension ref="A1:L995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>

</xml_diff>